<commit_message>
clean up development prints across files
</commit_message>
<xml_diff>
--- a/examples/example_income.xlsx
+++ b/examples/example_income.xlsx
@@ -24,7 +24,7 @@
     <t>Asset1</t>
   </si>
   <si>
-    <t>Asset2</t>
+    <t>Asset3</t>
   </si>
 </sst>
 </file>
@@ -869,7 +869,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>